<commit_message>
arrival read successful, with data cleaned
</commit_message>
<xml_diff>
--- a/Project 2/data_sets/arrival_09.xlsx
+++ b/Project 2/data_sets/arrival_09.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20346"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDB7A612-F8F9-4201-A113-C3748331D1DB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98F64D97-2753-4B02-874C-0E4F538A7EAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{6BDA6BB4-4E85-F84D-B3E1-69AFF496AF02}"/>
+    <workbookView xWindow="7730" yWindow="2100" windowWidth="28800" windowHeight="15460" xr2:uid="{6BDA6BB4-4E85-F84D-B3E1-69AFF496AF02}"/>
   </bookViews>
   <sheets>
     <sheet name="arrival" sheetId="1" r:id="rId1"/>
@@ -378,220 +378,220 @@
   <dimension ref="A1:A42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.125" customWidth="1"/>
+    <col min="1" max="1" width="11.08203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0.46509259259259261</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>0.4659490740740741</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>0.46637731481481487</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>0.46650462962962963</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>0.46695601851851848</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>0.46716435185185184</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>0.46739583333333329</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>0.46819444444444441</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>0.46866898148148151</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>0.46873842592592596</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>0.46878472222222217</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>0.46888888888888891</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>0.47003472222222226</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>0.47011574074074075</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>0.47027777777777779</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>0.47202546296296299</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>0.47332175925925929</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>0.47339120370370374</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>0.47351851851851851</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>0.4737615740740741</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>0.47396990740740735</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>0.47407407407407409</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
-        <v>0.4760416666666667</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+        <v>0.47395833333333331</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>0.47427083333333336</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>0.47655092592592596</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>0.47697916666666668</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>0.47849537037037032</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>0.47875000000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>0.47924768518518518</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>0.47994212962962962</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>0.48032407407407413</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>0.48033564814814816</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>0.48069444444444448</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>0.48078703703703707</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>0.48182870370370368</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <v>0.48195601851851855</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>0.48303240740740744</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>0.48318287037037039</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>0.48371527777777779</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>0.48390046296296302</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>0.48427083333333337</v>
       </c>

</xml_diff>